<commit_message>
Attendance fix + grades
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -599,21 +599,21 @@
   </sheetPr>
   <dimension ref="A1:DQ51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AQ1" activeCellId="0" sqref="AQ:AQ"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AQ23" activeCellId="0" sqref="AQ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="29.4285714285714"/>
     <col collapsed="false" hidden="true" max="4" min="3" style="1" width="0"/>
     <col collapsed="false" hidden="true" max="35" min="5" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="39" min="36" style="0" width="0"/>
     <col collapsed="false" hidden="true" max="41" min="40" style="3" width="0"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="3" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="3" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="3" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="3" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,6 +1485,7 @@
       <c r="AO6" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AP6" s="0"/>
       <c r="AQ6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1784,6 +1785,7 @@
       <c r="AO9" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AP9" s="0"/>
       <c r="AQ9" s="3" t="s">
         <v>7</v>
       </c>
@@ -2199,6 +2201,7 @@
       <c r="AO13" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AP13" s="0"/>
       <c r="AQ13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2805,6 +2808,8 @@
       <c r="AO19" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="AP19" s="0"/>
+      <c r="AQ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="n">
@@ -3000,6 +3005,7 @@
       <c r="AO21" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AP21" s="0"/>
       <c r="AQ21" s="3" t="s">
         <v>6</v>
       </c>
@@ -3179,7 +3185,7 @@
         <v>6</v>
       </c>
       <c r="AQ23" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4926,6 +4932,7 @@
       <c r="AO40" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AP40" s="0"/>
       <c r="AQ40" s="3" t="s">
         <v>6</v>
       </c>
@@ -5024,6 +5031,7 @@
       <c r="AP41" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="AQ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="n">
@@ -5481,6 +5489,7 @@
       <c r="AO46" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AP46" s="0"/>
       <c r="AQ46" s="3" t="s">
         <v>6</v>
       </c>
@@ -5734,6 +5743,7 @@
       <c r="AO49" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="AP49" s="0"/>
       <c r="AQ49" s="3" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Attendance + Grade fix
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="78">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -623,14 +623,14 @@
   </sheetPr>
   <dimension ref="A1:DQ51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AY51" activeCellId="0" sqref="AY51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AY8" activeCellId="0" sqref="AY8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="25.6479591836735"/>
     <col collapsed="false" hidden="true" max="4" min="3" style="1" width="0"/>
     <col collapsed="false" hidden="true" max="35" min="5" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="39" min="36" style="0" width="0"/>
@@ -639,7 +639,8 @@
     <col collapsed="false" hidden="true" max="47" min="47" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="49" min="48" style="0" width="0"/>
     <col collapsed="false" hidden="true" max="50" min="50" style="3" width="0"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="22.3622448979592"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="52" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,6 +1702,9 @@
       </c>
       <c r="AX7" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="AY7" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,6 +3485,9 @@
       <c r="AX23" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="AY23" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="n">

</xml_diff>

<commit_message>
iReviewer - Lecture 3
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="78">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -635,14 +635,14 @@
   </sheetPr>
   <dimension ref="A1:DQ51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BX51" activeCellId="0" sqref="BX51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CA36" activeCellId="0" sqref="CA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="25.3775510204082"/>
     <col collapsed="false" hidden="true" max="4" min="3" style="1" width="0"/>
     <col collapsed="false" hidden="true" max="35" min="5" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="39" min="36" style="0" width="0"/>
@@ -657,7 +657,11 @@
     <col collapsed="false" hidden="true" max="60" min="57" style="0" width="0"/>
     <col collapsed="false" hidden="true" max="62" min="61" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="75" min="63" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="43.8979591836735"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="0" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="80" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,6 +1189,12 @@
       <c r="BS2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BZ2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
@@ -1332,6 +1342,18 @@
       <c r="BS3" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BX3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA3" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
@@ -1496,6 +1518,15 @@
       <c r="BX4" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA4" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
@@ -1648,6 +1679,18 @@
       <c r="BS5" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BX5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA5" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
@@ -1801,6 +1844,15 @@
       <c r="BX6" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BY6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA6" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="n">
@@ -1965,6 +2017,15 @@
       <c r="BX7" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BY7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA7" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="n">
@@ -2122,6 +2183,15 @@
       </c>
       <c r="BR8" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="BY8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA8" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,6 +2336,9 @@
       <c r="BX9" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BZ9" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="n">
@@ -2586,6 +2659,15 @@
       <c r="BX11" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BY11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA11" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="n">
@@ -2750,6 +2832,15 @@
       <c r="BX12" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA12" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="n">
@@ -2901,6 +2992,15 @@
       <c r="BX13" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA13" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="n">
@@ -3051,6 +3151,12 @@
       <c r="BX14" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ14" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="n">
@@ -3204,6 +3310,15 @@
       <c r="BX15" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BY15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA15" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="n">
@@ -3368,6 +3483,15 @@
       <c r="BX16" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA16" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="n">
@@ -3527,6 +3651,9 @@
       <c r="BS17" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BZ17" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="n">
@@ -3690,6 +3817,15 @@
       </c>
       <c r="BX18" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="BY18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA18" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3938,6 +4074,18 @@
       <c r="BS20" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BX20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA20" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="n">
@@ -4090,6 +4238,15 @@
       </c>
       <c r="BX21" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="BY21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA21" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,6 +4491,15 @@
       <c r="BX23" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA23" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="n">
@@ -4498,6 +4664,15 @@
       <c r="BX24" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA24" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="n">
@@ -4662,6 +4837,15 @@
       <c r="BX25" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA25" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="n">
@@ -4818,6 +5002,15 @@
       <c r="BS26" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA26" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="n">
@@ -4982,6 +5175,15 @@
       <c r="BX27" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA27" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="n">
@@ -5144,6 +5346,15 @@
       <c r="BX28" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA28" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="n">
@@ -5308,6 +5519,12 @@
       <c r="BX29" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ29" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="n">
@@ -5472,6 +5689,15 @@
       <c r="BX30" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA30" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="n">
@@ -5636,6 +5862,15 @@
       <c r="BX31" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY31" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ31" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA31" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="n">
@@ -5800,6 +6035,15 @@
       <c r="BX32" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA32" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="n">
@@ -5961,6 +6205,15 @@
       </c>
       <c r="BX33" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="BY33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA33" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6260,6 +6513,9 @@
       <c r="BS35" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BZ35" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="n">
@@ -6420,6 +6676,15 @@
       <c r="BX36" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BY36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA36" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="n">
@@ -6578,6 +6843,15 @@
       <c r="BX37" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA37" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="n">
@@ -6734,6 +7008,12 @@
       <c r="BX38" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BY38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ38" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="n">
@@ -6892,6 +7172,15 @@
       <c r="BX39" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA39" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="n">
@@ -7198,6 +7487,15 @@
       <c r="BX41" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BY41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA41" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="n">
@@ -7474,6 +7772,15 @@
         <v>6</v>
       </c>
       <c r="BX43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA43" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7623,6 +7930,9 @@
       <c r="BX44" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BZ44" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="n">
@@ -7776,6 +8086,15 @@
       <c r="BX45" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA45" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="n">
@@ -7915,6 +8234,9 @@
       <c r="BR46" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="BZ46" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="n">
@@ -8069,6 +8391,15 @@
       <c r="BX47" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA47" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="n">
@@ -8211,6 +8542,12 @@
       </c>
       <c r="BX48" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="BZ48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA48" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8455,6 +8792,15 @@
       <c r="BX50" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="BY50" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ50" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA50" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="n">
@@ -8554,6 +8900,9 @@
         <v>7</v>
       </c>
       <c r="BS51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ51" s="0" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assignment 9 - Marks
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="78">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -635,14 +635,14 @@
   </sheetPr>
   <dimension ref="A1:DQ51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CE51" activeCellId="0" sqref="CE51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CE29" activeCellId="0" sqref="CE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.4897959183673"/>
     <col collapsed="false" hidden="true" max="4" min="3" style="1" width="0"/>
     <col collapsed="false" hidden="true" max="35" min="5" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="39" min="36" style="0" width="0"/>
@@ -657,7 +657,8 @@
     <col collapsed="false" hidden="true" max="60" min="57" style="0" width="0"/>
     <col collapsed="false" hidden="true" max="62" min="61" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="82" min="63" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="29.3112244897959"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="84" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,6 +1532,9 @@
       </c>
       <c r="CD4" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="CE4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4577,6 +4581,9 @@
       <c r="CD23" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CE23" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="n">
@@ -5100,6 +5107,9 @@
       <c r="CA26" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CE26" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="n">
@@ -5450,6 +5460,9 @@
       <c r="CA28" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CE28" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="n">
@@ -5621,6 +5634,9 @@
         <v>6</v>
       </c>
       <c r="CD29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CE29" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7939,6 +7955,9 @@
         <v>6</v>
       </c>
       <c r="CA43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CE43" s="0" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Forangram - Part 2 done
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="78">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -635,14 +635,14 @@
   </sheetPr>
   <dimension ref="A1:DQ51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CE29" activeCellId="0" sqref="CE29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CD20" activeCellId="0" sqref="CD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="11.5204081632653"/>
     <col collapsed="false" hidden="true" max="4" min="3" style="1" width="0"/>
     <col collapsed="false" hidden="true" max="35" min="5" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="39" min="36" style="0" width="0"/>
@@ -656,9 +656,10 @@
     <col collapsed="false" hidden="true" max="56" min="56" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="60" min="57" style="0" width="0"/>
     <col collapsed="false" hidden="true" max="62" min="61" style="3" width="0"/>
-    <col collapsed="false" hidden="true" max="82" min="63" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="84" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="true" max="81" min="63" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="83" min="82" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="0" width="35.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="85" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,6 +1537,9 @@
       <c r="CE4" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CF4" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
@@ -2369,6 +2373,9 @@
       <c r="CE9" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF9" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="n">
@@ -2704,6 +2711,9 @@
       <c r="CE11" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF11" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="n">
@@ -2883,6 +2893,9 @@
       <c r="CE12" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF12" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="n">
@@ -3049,6 +3062,9 @@
       <c r="CE13" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF13" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="n">
@@ -3379,6 +3395,9 @@
       <c r="CE15" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF15" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="n">
@@ -3556,6 +3575,9 @@
         <v>6</v>
       </c>
       <c r="CE16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CF16" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4159,6 +4181,15 @@
         <v>7</v>
       </c>
       <c r="CA20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CD20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF20" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5289,6 +5320,9 @@
       <c r="CE27" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF27" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="n">
@@ -5818,6 +5852,9 @@
       <c r="CE30" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF30" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="n">
@@ -5997,6 +6034,9 @@
       <c r="CE31" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CF31" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="n">
@@ -6176,6 +6216,9 @@
       <c r="CE32" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CF32" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="n">
@@ -6353,6 +6396,9 @@
       <c r="CE33" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF33" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="n">
@@ -6504,6 +6550,9 @@
         <v>7</v>
       </c>
       <c r="CE34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF34" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6666,6 +6715,9 @@
       <c r="CE35" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF35" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="n">
@@ -7008,6 +7060,9 @@
       <c r="CE37" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF37" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="n">
@@ -7173,6 +7228,9 @@
       <c r="CD38" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CF38" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="n">
@@ -7343,6 +7401,9 @@
       <c r="CD39" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CF39" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="n">
@@ -7499,6 +7560,9 @@
         <v>6</v>
       </c>
       <c r="CE40" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF40" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -8113,6 +8177,9 @@
       <c r="CD44" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF44" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="n">
@@ -8426,6 +8493,9 @@
       <c r="CD46" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CF46" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="n">
@@ -8595,6 +8665,9 @@
       <c r="CE47" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CF47" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="n">
@@ -8745,6 +8818,9 @@
         <v>7</v>
       </c>
       <c r="CD48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF48" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -9112,6 +9188,9 @@
       <c r="CD51" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="CF51" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Attendance + Project list
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2905" uniqueCount="78">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -639,14 +639,14 @@
   </sheetPr>
   <dimension ref="A1:DQ51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CV42" activeCellId="0" sqref="CV42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CZ50" activeCellId="0" sqref="CZ50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="19.5714285714286"/>
     <col collapsed="false" hidden="true" max="4" min="3" style="1" width="0"/>
     <col collapsed="false" hidden="true" max="35" min="5" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="39" min="36" style="0" width="0"/>
@@ -662,8 +662,9 @@
     <col collapsed="false" hidden="true" max="62" min="61" style="3" width="0"/>
     <col collapsed="false" hidden="true" max="95" min="63" style="0" width="0"/>
     <col collapsed="false" hidden="true" max="99" min="96" style="3" width="0"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="true" max="103" min="100" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="104" min="104" style="0" width="43.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="105" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,6 +1232,12 @@
       <c r="CV2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
@@ -1409,6 +1416,9 @@
       <c r="CV3" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ3" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
@@ -1622,6 +1632,12 @@
         <v>6</v>
       </c>
       <c r="CV4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CY4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ4" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1807,6 +1823,9 @@
       <c r="CV5" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ5" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
@@ -2007,6 +2026,12 @@
       <c r="CV6" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ6" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="n">
@@ -2210,6 +2235,9 @@
       </c>
       <c r="CV7" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="CZ7" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,6 +2413,9 @@
       <c r="CS8" s="0"/>
       <c r="CT8" s="15"/>
       <c r="CU8" s="15"/>
+      <c r="CZ8" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="n">
@@ -2563,6 +2594,12 @@
       <c r="CV9" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ9" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="n">
@@ -2726,6 +2763,9 @@
       <c r="CS10" s="0"/>
       <c r="CT10" s="15"/>
       <c r="CU10" s="15"/>
+      <c r="CZ10" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="n">
@@ -2939,6 +2979,9 @@
       <c r="CV11" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ11" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="n">
@@ -3154,6 +3197,12 @@
       <c r="CV12" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ12" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="n">
@@ -3351,6 +3400,9 @@
       <c r="CV13" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ13" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="n">
@@ -3539,6 +3591,9 @@
       <c r="CV14" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ14" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="n">
@@ -3737,6 +3792,12 @@
       <c r="CV15" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ15" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="n">
@@ -3950,6 +4011,12 @@
         <v>6</v>
       </c>
       <c r="CV16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CY16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ16" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4127,6 +4194,9 @@
       <c r="CV17" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ17" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="n">
@@ -4337,6 +4407,12 @@
         <v>6</v>
       </c>
       <c r="CV18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CY18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ18" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4644,6 +4720,12 @@
       <c r="CV20" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ20" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="n">
@@ -4830,6 +4912,9 @@
       </c>
       <c r="CV21" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="CZ21" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5129,6 +5214,9 @@
       <c r="CV23" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ23" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="n">
@@ -5344,6 +5432,9 @@
       <c r="CV24" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ24" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="n">
@@ -5559,6 +5650,9 @@
       <c r="CV25" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ25" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="n">
@@ -5753,6 +5847,9 @@
       <c r="CV26" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ26" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="n">
@@ -5963,6 +6060,12 @@
       <c r="CV27" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CZ27" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="n">
@@ -6170,6 +6273,9 @@
       <c r="CV28" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ28" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="n">
@@ -6379,6 +6485,9 @@
       <c r="CV29" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ29" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="n">
@@ -6594,6 +6703,12 @@
       <c r="CV30" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ30" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="n">
@@ -6809,6 +6924,12 @@
       <c r="CV31" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ31" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="n">
@@ -7024,6 +7145,12 @@
       <c r="CV32" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ32" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="n">
@@ -7237,6 +7364,12 @@
       <c r="CV33" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CZ33" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="n">
@@ -7425,6 +7558,9 @@
       </c>
       <c r="CV34" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="CZ34" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7599,6 +7735,12 @@
       <c r="CS35" s="0"/>
       <c r="CT35" s="15"/>
       <c r="CU35" s="15"/>
+      <c r="CY35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ35" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="n">
@@ -7798,6 +7940,9 @@
       <c r="CV36" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ36" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="n">
@@ -8004,6 +8149,9 @@
       <c r="CV37" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ37" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="n">
@@ -8205,6 +8353,9 @@
       <c r="CV38" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ38" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="n">
@@ -8411,6 +8562,9 @@
       <c r="CV39" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ39" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="n">
@@ -8602,6 +8756,9 @@
       <c r="CV40" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ40" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="n">
@@ -8804,6 +8961,12 @@
       <c r="CV41" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ41" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="n">
@@ -8940,6 +9103,9 @@
       <c r="CS42" s="0"/>
       <c r="CT42" s="15"/>
       <c r="CU42" s="15"/>
+      <c r="CZ42" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="n">
@@ -9136,6 +9302,9 @@
       </c>
       <c r="CV43" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="CZ43" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9319,6 +9488,12 @@
       <c r="CV44" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="CZ44" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="n">
@@ -9520,6 +9695,9 @@
       <c r="CV45" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ45" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="n">
@@ -9681,6 +9859,9 @@
       <c r="CS46" s="0"/>
       <c r="CT46" s="15"/>
       <c r="CU46" s="15"/>
+      <c r="CZ46" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="n">
@@ -9886,6 +10067,12 @@
       <c r="CV47" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CY47" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="CZ47" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="n">
@@ -10062,6 +10249,9 @@
       </c>
       <c r="CV48" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="CZ48" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10358,6 +10548,9 @@
       <c r="CV50" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="CZ50" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="n">
@@ -10473,6 +10666,9 @@
       </c>
       <c r="CV51" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="CZ51" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>